<commit_message>
Status and charts updated
</commit_message>
<xml_diff>
--- a/Spreadsheets/Corona Stats of Pakistan.xlsx
+++ b/Spreadsheets/Corona Stats of Pakistan.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10307"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Muhammad/Documents/Github/Corona stats of Pakistan/Spreadsheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F59BB9-61BF-E147-8C40-72C74E404B96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
   <si>
     <t>CityNames</t>
   </si>
@@ -91,12 +97,36 @@
     <t>215</t>
   </si>
   <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>2,672</t>
+  </si>
+  <si>
+    <t>1,452</t>
+  </si>
+  <si>
+    <t>744</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
     <t>2020-04-09</t>
   </si>
   <si>
     <t>2020-04-10</t>
   </si>
   <si>
+    <t>2020-04-13</t>
+  </si>
+  <si>
     <t>Recovered</t>
   </si>
   <si>
@@ -158,13 +188,34 @@
   </si>
   <si>
     <t>54,706</t>
+  </si>
+  <si>
+    <t>1,097</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>3,233</t>
+  </si>
+  <si>
+    <t>65,114</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -227,6 +278,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -273,7 +332,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -305,9 +364,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -339,6 +416,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -514,14 +609,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -538,7 +642,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -546,16 +650,16 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -563,16 +667,16 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -580,16 +684,16 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -597,16 +701,16 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -614,16 +718,16 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -631,16 +735,16 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -648,16 +752,16 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -665,16 +769,16 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="E9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -682,16 +786,16 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -699,16 +803,16 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -716,16 +820,16 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -733,16 +837,16 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -750,16 +854,16 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -767,13 +871,132 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
         <v>26</v>
       </c>
-      <c r="D15" t="s">
-        <v>33</v>
-      </c>
-      <c r="E15" t="s">
-        <v>47</v>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
+        <v>34</v>
+      </c>
+      <c r="D18" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+      <c r="D22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chart updated with latest stats
</commit_message>
<xml_diff>
--- a/Spreadsheets/Corona Stats of Pakistan.xlsx
+++ b/Spreadsheets/Corona Stats of Pakistan.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10307"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Muhammad/Documents/Github/Corona stats of Pakistan/Spreadsheets/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F59BB9-61BF-E147-8C40-72C74E404B96}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
   <si>
     <t>CityNames</t>
   </si>
@@ -118,6 +112,21 @@
     <t>224</t>
   </si>
   <si>
+    <t>2,881</t>
+  </si>
+  <si>
+    <t>1,518</t>
+  </si>
+  <si>
+    <t>800</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>233</t>
+  </si>
+  <si>
     <t>2020-04-09</t>
   </si>
   <si>
@@ -127,6 +136,9 @@
     <t>2020-04-13</t>
   </si>
   <si>
+    <t>2020-04-14</t>
+  </si>
+  <si>
     <t>Recovered</t>
   </si>
   <si>
@@ -209,13 +221,34 @@
   </si>
   <si>
     <t>65,114</t>
+  </si>
+  <si>
+    <t>1,378</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>3,157</t>
+  </si>
+  <si>
+    <t>69,928</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -278,14 +311,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -332,7 +357,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -364,27 +389,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -416,24 +423,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -609,23 +598,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,7 +622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -650,16 +630,16 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -667,16 +647,16 @@
         <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -684,16 +664,16 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -701,16 +681,16 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -718,16 +698,16 @@
         <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -735,16 +715,16 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -752,16 +732,16 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -769,16 +749,16 @@
         <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -786,16 +766,16 @@
         <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -803,16 +783,16 @@
         <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -820,16 +800,16 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D12" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -837,16 +817,16 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -854,16 +834,16 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -871,16 +851,16 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D15" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -888,16 +868,16 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="E16" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -905,16 +885,16 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D17" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -922,16 +902,16 @@
         <v>27</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D18" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -939,16 +919,16 @@
         <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D19" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -956,16 +936,16 @@
         <v>29</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -973,16 +953,16 @@
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -990,13 +970,132 @@
         <v>31</v>
       </c>
       <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" t="s">
+        <v>40</v>
+      </c>
+      <c r="D23" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
         <v>34</v>
       </c>
-      <c r="D22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E22" t="s">
-        <v>62</v>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>9</v>
+      </c>
+      <c r="B27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>40</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" t="s">
+        <v>40</v>
+      </c>
+      <c r="D29" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
apr 15 2020 latest stats
</commit_message>
<xml_diff>
--- a/Spreadsheets/Corona Stats of Pakistan.xlsx
+++ b/Spreadsheets/Corona Stats of Pakistan.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Muhammad/Documents/Github/Corona stats of Pakistan/Spreadsheets/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE67E496-BA1F-A440-9E9C-8C6C5ACDF53A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="89">
   <si>
     <t>CityNames</t>
   </si>
@@ -22,6 +28,9 @@
     <t>CityWiseCounts</t>
   </si>
   <si>
+    <t>ConfirmedCases</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -127,6 +136,27 @@
     <t>233</t>
   </si>
   <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>2,945</t>
+  </si>
+  <si>
+    <t>865</t>
+  </si>
+  <si>
+    <t>240</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>5,988</t>
+  </si>
+  <si>
     <t>2020-04-09</t>
   </si>
   <si>
@@ -139,6 +169,9 @@
     <t>2020-04-14</t>
   </si>
   <si>
+    <t>2020-04-15</t>
+  </si>
+  <si>
     <t>Recovered</t>
   </si>
   <si>
@@ -226,9 +259,6 @@
     <t>1,378</t>
   </si>
   <si>
-    <t>46</t>
-  </si>
-  <si>
     <t>96</t>
   </si>
   <si>
@@ -242,13 +272,28 @@
   </si>
   <si>
     <t>69,928</t>
+  </si>
+  <si>
+    <t>1,446</t>
+  </si>
+  <si>
+    <t>272</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>3,280</t>
+  </si>
+  <si>
+    <t>73,439</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,6 +356,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -357,7 +410,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -389,9 +442,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -423,6 +494,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -598,14 +687,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -621,481 +718,624 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>50</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="E3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>51</v>
+      </c>
+      <c r="F3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>52</v>
+      </c>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
       </c>
       <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" t="s">
+      <c r="F11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
         <v>46</v>
       </c>
-      <c r="E7" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" t="s">
+      <c r="E13" t="s">
+        <v>54</v>
+      </c>
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" t="s">
-        <v>45</v>
-      </c>
-      <c r="E13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
       <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
         <v>46</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>55</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>52</v>
+      </c>
+      <c r="F18" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
         <v>47</v>
       </c>
-      <c r="E15" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s">
-        <v>25</v>
-      </c>
-      <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" t="s">
-        <v>26</v>
-      </c>
-      <c r="C17" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17" t="s">
-        <v>42</v>
-      </c>
-      <c r="E17" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>27</v>
-      </c>
-      <c r="C18" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C20" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" t="s">
-        <v>46</v>
-      </c>
       <c r="E21" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+        <v>55</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D22" t="s">
         <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+        <v>56</v>
+      </c>
+      <c r="F22" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E23" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>51</v>
+      </c>
+      <c r="F24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>48</v>
+      </c>
+      <c r="E26" t="s">
+        <v>53</v>
+      </c>
+      <c r="F26" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>48</v>
+      </c>
+      <c r="E27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F27" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+      <c r="D28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
+        <v>55</v>
+      </c>
+      <c r="F28" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>48</v>
+      </c>
+      <c r="E29" t="s">
+        <v>56</v>
+      </c>
+      <c r="F29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="s">
+        <v>44</v>
+      </c>
+      <c r="D31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" t="s">
+        <v>51</v>
+      </c>
+      <c r="F31" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" t="s">
+        <v>52</v>
+      </c>
+      <c r="F32" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33" t="s">
         <v>40</v>
       </c>
-      <c r="D23" t="s">
+      <c r="C33" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
         <v>41</v>
       </c>
-      <c r="E23" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
-        <v>6</v>
-      </c>
-      <c r="B24" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" t="s">
-        <v>40</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C34" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
         <v>42</v>
       </c>
-      <c r="E24" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" t="s">
+      <c r="C35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
         <v>43</v>
       </c>
-      <c r="E25" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" t="s">
+      <c r="C36" t="s">
         <v>44</v>
       </c>
-      <c r="E26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="A28" t="s">
-        <v>10</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" t="s">
-        <v>47</v>
-      </c>
-      <c r="E29" t="s">
-        <v>75</v>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>